<commit_message>
update hide/show columns features
</commit_message>
<xml_diff>
--- a/upload/file/plan/P/P-Ke Hoach San Xuat Order 120_(4.19).xlsx
+++ b/upload/file/plan/P/P-Ke Hoach San Xuat Order 120_(4.19).xlsx
@@ -16,7 +16,7 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -9473,9 +9473,6 @@
     <t>VaiChinh</t>
   </si>
   <si>
-    <t>VaiLot</t>
-  </si>
-  <si>
     <t>VaiVien</t>
   </si>
   <si>
@@ -9495,15 +9492,6 @@
   </si>
   <si>
     <t>TTVaiChinh</t>
-  </si>
-  <si>
-    <t>DMVaiLot</t>
-  </si>
-  <si>
-    <t>SLVaiLot</t>
-  </si>
-  <si>
-    <t>TTVaiLot</t>
   </si>
   <si>
     <t>DMVaiVien</t>
@@ -9612,6 +9600,18 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>VaiLot6</t>
+  </si>
+  <si>
+    <t>DMVaiLot6</t>
+  </si>
+  <si>
+    <t>SLVaiLot6</t>
+  </si>
+  <si>
+    <t>TTVaiLot6</t>
   </si>
 </sst>
 </file>
@@ -21573,7 +21573,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="DATE">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable10" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="DATE">
   <location ref="A3:N47" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="63">
     <pivotField showAll="0"/>
@@ -22355,7 +22355,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -22368,9 +22368,9 @@
   </sheetPr>
   <dimension ref="A1:CB613"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BX1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE2" sqref="AE2"/>
+      <selection pane="bottomLeft" activeCell="AQ5" sqref="AQ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -22444,13 +22444,13 @@
   <sheetData>
     <row r="1" spans="1:80" s="94" customFormat="1" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>434</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>418</v>
@@ -22471,7 +22471,7 @@
         <v>420</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="K1" s="22" t="s">
         <v>421</v>
@@ -22534,7 +22534,7 @@
         <v>432</v>
       </c>
       <c r="AE1" s="22" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="AF1" s="22" t="s">
         <v>13</v>
@@ -22552,136 +22552,136 @@
         <v>444</v>
       </c>
       <c r="AK1" s="97" t="s">
+        <v>449</v>
+      </c>
+      <c r="AL1" s="97" t="s">
         <v>450</v>
       </c>
-      <c r="AL1" s="97" t="s">
+      <c r="AM1" s="97" t="s">
         <v>451</v>
       </c>
-      <c r="AM1" s="97" t="s">
+      <c r="AN1" s="95" t="s">
+        <v>488</v>
+      </c>
+      <c r="AO1" s="95" t="s">
+        <v>489</v>
+      </c>
+      <c r="AP1" s="95" t="s">
+        <v>490</v>
+      </c>
+      <c r="AQ1" s="95" t="s">
+        <v>491</v>
+      </c>
+      <c r="AR1" s="97" t="s">
+        <v>445</v>
+      </c>
+      <c r="AS1" s="97" t="s">
         <v>452</v>
       </c>
-      <c r="AN1" s="95" t="s">
-        <v>445</v>
-      </c>
-      <c r="AO1" s="95" t="s">
+      <c r="AT1" s="97" t="s">
         <v>453</v>
       </c>
-      <c r="AP1" s="95" t="s">
+      <c r="AU1" s="97" t="s">
         <v>454</v>
       </c>
-      <c r="AQ1" s="95" t="s">
+      <c r="AV1" s="95" t="s">
+        <v>446</v>
+      </c>
+      <c r="AW1" s="95" t="s">
         <v>455</v>
       </c>
-      <c r="AR1" s="97" t="s">
-        <v>446</v>
-      </c>
-      <c r="AS1" s="97" t="s">
+      <c r="AX1" s="95" t="s">
         <v>456</v>
       </c>
-      <c r="AT1" s="97" t="s">
+      <c r="AY1" s="95" t="s">
         <v>457</v>
       </c>
-      <c r="AU1" s="97" t="s">
+      <c r="AZ1" s="97" t="s">
+        <v>447</v>
+      </c>
+      <c r="BA1" s="97" t="s">
         <v>458</v>
       </c>
-      <c r="AV1" s="95" t="s">
-        <v>447</v>
-      </c>
-      <c r="AW1" s="95" t="s">
+      <c r="BB1" s="97" t="s">
         <v>459</v>
       </c>
-      <c r="AX1" s="95" t="s">
+      <c r="BC1" s="97" t="s">
         <v>460</v>
       </c>
-      <c r="AY1" s="95" t="s">
+      <c r="BD1" s="95" t="s">
+        <v>448</v>
+      </c>
+      <c r="BE1" s="95" t="s">
         <v>461</v>
       </c>
-      <c r="AZ1" s="97" t="s">
-        <v>448</v>
-      </c>
-      <c r="BA1" s="97" t="s">
+      <c r="BF1" s="96" t="s">
         <v>462</v>
       </c>
-      <c r="BB1" s="97" t="s">
+      <c r="BG1" s="95" t="s">
         <v>463</v>
       </c>
-      <c r="BC1" s="97" t="s">
+      <c r="BH1" s="97" t="s">
         <v>464</v>
       </c>
-      <c r="BD1" s="95" t="s">
-        <v>449</v>
-      </c>
-      <c r="BE1" s="95" t="s">
+      <c r="BI1" s="97" t="s">
         <v>465</v>
       </c>
-      <c r="BF1" s="96" t="s">
+      <c r="BJ1" s="98" t="s">
         <v>466</v>
       </c>
-      <c r="BG1" s="95" t="s">
+      <c r="BK1" s="97" t="s">
         <v>467</v>
       </c>
-      <c r="BH1" s="97" t="s">
+      <c r="BL1" s="95" t="s">
         <v>468</v>
       </c>
-      <c r="BI1" s="97" t="s">
+      <c r="BM1" s="95" t="s">
         <v>469</v>
       </c>
-      <c r="BJ1" s="98" t="s">
+      <c r="BN1" s="95" t="s">
         <v>470</v>
       </c>
-      <c r="BK1" s="97" t="s">
+      <c r="BO1" s="95" t="s">
         <v>471</v>
       </c>
-      <c r="BL1" s="95" t="s">
+      <c r="BP1" s="97" t="s">
         <v>472</v>
       </c>
-      <c r="BM1" s="95" t="s">
+      <c r="BQ1" s="97" t="s">
         <v>473</v>
       </c>
-      <c r="BN1" s="95" t="s">
+      <c r="BR1" s="98" t="s">
         <v>474</v>
       </c>
-      <c r="BO1" s="95" t="s">
+      <c r="BS1" s="97" t="s">
         <v>475</v>
       </c>
-      <c r="BP1" s="97" t="s">
+      <c r="BT1" s="95" t="s">
         <v>476</v>
       </c>
-      <c r="BQ1" s="97" t="s">
+      <c r="BU1" s="95" t="s">
         <v>477</v>
       </c>
-      <c r="BR1" s="98" t="s">
+      <c r="BV1" s="95" t="s">
         <v>478</v>
       </c>
-      <c r="BS1" s="97" t="s">
+      <c r="BW1" s="95" t="s">
         <v>479</v>
-      </c>
-      <c r="BT1" s="95" t="s">
-        <v>480</v>
-      </c>
-      <c r="BU1" s="95" t="s">
-        <v>481</v>
-      </c>
-      <c r="BV1" s="95" t="s">
-        <v>482</v>
-      </c>
-      <c r="BW1" s="95" t="s">
-        <v>483</v>
       </c>
       <c r="BX1" s="93" t="s">
         <v>367</v>
       </c>
       <c r="BY1" s="93" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="BZ1" s="93" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="CA1" s="93" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="CB1" s="93" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2" spans="1:80" s="24" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>